<commit_message>
Rough final no buttons portals fixed
</commit_message>
<xml_diff>
--- a/map1.xlsx
+++ b/map1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arpit\coding\twiet\schoolSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{224EA72A-6C45-4B6D-9436-E99BBDF05D01}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E81F15-2251-4F8A-A7C1-110B2A148C85}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -407,8 +407,8 @@
   </sheetPr>
   <dimension ref="G1:CU113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="BS39" sqref="BS39"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
+      <selection activeCell="BN29" sqref="BN29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1024,7 +1024,8 @@
       <c r="BB26" s="11"/>
       <c r="BC26" s="11"/>
       <c r="BD26" s="4"/>
-      <c r="BQ26" s="4"/>
+      <c r="BP26" s="5"/>
+      <c r="BQ26" s="5"/>
       <c r="BR26" s="5"/>
       <c r="BS26" s="5"/>
       <c r="BT26" s="5"/>
@@ -1039,7 +1040,8 @@
       <c r="BB27" s="11"/>
       <c r="BC27" s="11"/>
       <c r="BD27" s="4"/>
-      <c r="BQ27" s="4"/>
+      <c r="BP27" s="5"/>
+      <c r="BQ27" s="5"/>
       <c r="BR27" s="5"/>
       <c r="BS27" s="5"/>
       <c r="BT27" s="5"/>
@@ -1054,7 +1056,8 @@
       <c r="BB28" s="10"/>
       <c r="BC28" s="10"/>
       <c r="BD28" s="10"/>
-      <c r="BQ28" s="4"/>
+      <c r="BP28" s="5"/>
+      <c r="BQ28" s="5"/>
       <c r="BR28" s="5"/>
       <c r="BS28" s="5"/>
       <c r="BT28" s="5"/>
@@ -1072,7 +1075,7 @@
       <c r="BK29" s="4"/>
       <c r="BL29" s="4"/>
       <c r="BM29" s="4"/>
-      <c r="BN29" s="4"/>
+      <c r="BN29" s="20"/>
       <c r="BQ29" s="4"/>
       <c r="BR29" s="4"/>
       <c r="BS29" s="4"/>

</xml_diff>